<commit_message>
Added sync methods. Updated md files.
</commit_message>
<xml_diff>
--- a/samples/SampleTest/YahooWeather/Resources/Test_NewYork.xlsx
+++ b/samples/SampleTest/YahooWeather/Resources/Test_NewYork.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitProjects\CsvBasedWebTest\sample\SampleTest\YahooWeather\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitProjects\Tatami-dotnet\samples\SampleTest\YahooWeather\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1316,11 +1316,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1490,10 +1488,10 @@
       <c r="G5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J5" s="15" t="s">
@@ -1595,16 +1593,16 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="16"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17" t="s">
         <v>40</v>
@@ -1620,386 +1618,6 @@
       </c>
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="16"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="16"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="15"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="16"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="16"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="16"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="16"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="17"/>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="2"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="16"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="16"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="17"/>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="16"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="17"/>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="16"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="2"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="15"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="16"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="16"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="16"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="16"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="16"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="17"/>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29" s="2"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>

</xml_diff>